<commit_message>
ABM de articulos ahora puede dar las altas. El remito se genera con el Nro del mismo en la planilla.
</commit_message>
<xml_diff>
--- a/DOCS/REMITO_Master.xlsx
+++ b/DOCS/REMITO_Master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORKS\CAPELLO SOMBREROS\APPLICATION\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF94212-76E5-4601-A65B-D00900B1E769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3EA12E-EAA4-42B5-A506-2033A79D9F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>+</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>CAPELLO</t>
+  </si>
+  <si>
+    <t>REMITO DE MERCADERÍA EN CONSIGNACIÓN</t>
+  </si>
+  <si>
+    <t>Nro.00000</t>
   </si>
 </sst>
 </file>
@@ -123,7 +129,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="_ [$€-2]\ * #,##0.00_ ;_ [$€-2]\ * \-#,##0.00_ ;_ [$€-2]\ * &quot;-&quot;??_ "/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -168,6 +174,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Copperplate Gothic Bold"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -500,19 +512,18 @@
     <xf numFmtId="42" fontId="5" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -530,8 +541,11 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -843,7 +857,7 @@
   <dimension ref="A1:AR858"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G3"/>
+      <selection activeCell="A8" sqref="A8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -878,20 +892,20 @@
       <c r="E2" s="52"/>
       <c r="F2" s="52"/>
       <c r="G2" s="53"/>
-      <c r="H2" s="69">
+      <c r="H2" s="56">
         <v>0.7</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:17" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -905,36 +919,36 @@
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="63" t="s">
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="57"/>
+      <c r="G5" s="59"/>
       <c r="H5" s="38">
         <v>445</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="65"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="64"/>
       <c r="F6" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="64" t="s">
+      <c r="G6" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="65"/>
+      <c r="H6" s="64"/>
     </row>
     <row r="7" spans="1:17" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
@@ -947,14 +961,18 @@
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="60"/>
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="62"/>
+      <c r="A8" s="68" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="69"/>
+      <c r="H8" s="57" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:17" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
@@ -1441,8 +1459,8 @@
       <c r="C43" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D43" s="58"/>
-      <c r="E43" s="59"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="61"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="5"/>
@@ -1521,11 +1539,11 @@
   <mergeCells count="7">
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="D43:E43"/>
-    <mergeCell ref="A8:H8"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A8:G8"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
Se ocultan datos sensibles
</commit_message>
<xml_diff>
--- a/DOCS/REMITO_Master.xlsx
+++ b/DOCS/REMITO_Master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORKS\CAPELLO SOMBREROS\APPLICATION\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3EA12E-EAA4-42B5-A506-2033A79D9F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDBC15A-8D47-4BD0-A58B-F05BE8B51854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>+</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Fecha de retiro</t>
   </si>
   <si>
-    <t>AVILA Y ZARATE 2222 - TEL: 351 5 080336</t>
-  </si>
-  <si>
     <t>BOCA No.</t>
   </si>
   <si>
@@ -95,16 +92,7 @@
     <t>Vendido</t>
   </si>
   <si>
-    <t>351 3 081170</t>
-  </si>
-  <si>
     <t>devueltos</t>
-  </si>
-  <si>
-    <t>OPTICA TALAR de GASTON SIGUIENZA</t>
-  </si>
-  <si>
-    <t>AV. TISSERA 2205 - TALAR DE MENDIOLAZA</t>
   </si>
   <si>
     <t>Sombreros, Gorros y accesorios</t>
@@ -857,7 +845,7 @@
   <dimension ref="A1:AR858"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:G8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -882,11 +870,11 @@
     </row>
     <row r="2" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="51" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="52" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D2" s="52"/>
       <c r="E2" s="52"/>
@@ -897,9 +885,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
-        <v>6</v>
-      </c>
+      <c r="A3" s="58"/>
       <c r="B3" s="59"/>
       <c r="C3" s="59"/>
       <c r="D3" s="59"/>
@@ -919,35 +905,27 @@
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="65" t="s">
-        <v>21</v>
-      </c>
+      <c r="A5" s="65"/>
       <c r="B5" s="66"/>
       <c r="C5" s="66"/>
       <c r="D5" s="66"/>
       <c r="E5" s="64"/>
       <c r="F5" s="62" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G5" s="59"/>
-      <c r="H5" s="38">
-        <v>445</v>
-      </c>
+      <c r="H5" s="38"/>
     </row>
     <row r="6" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="67" t="s">
-        <v>22</v>
-      </c>
+      <c r="A6" s="67"/>
       <c r="B6" s="66"/>
       <c r="C6" s="66"/>
       <c r="D6" s="66"/>
       <c r="E6" s="64"/>
       <c r="F6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="63" t="s">
-        <v>19</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="G6" s="63"/>
       <c r="H6" s="64"/>
     </row>
     <row r="7" spans="1:17" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -962,7 +940,7 @@
     </row>
     <row r="8" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="68" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B8" s="69"/>
       <c r="C8" s="69"/>
@@ -971,33 +949,33 @@
       <c r="F8" s="69"/>
       <c r="G8" s="69"/>
       <c r="H8" s="57" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="13" t="s">
+      <c r="D9" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="E9" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="F9" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="28" t="s">
+      <c r="H9" s="30" t="s">
         <v>14</v>
-      </c>
-      <c r="H9" s="30" t="s">
-        <v>15</v>
       </c>
       <c r="I9" s="22"/>
       <c r="Q9" s="2"/>
@@ -1366,7 +1344,7 @@
     <row r="35" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A35" s="20"/>
       <c r="C35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="41">
@@ -1379,7 +1357,7 @@
       <c r="A36" s="11"/>
       <c r="B36" s="18"/>
       <c r="C36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="41">
@@ -1391,7 +1369,7 @@
       <c r="A37" s="11"/>
       <c r="B37" s="18"/>
       <c r="C37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="41">

</xml_diff>

<commit_message>
Recarga de articulos y clientes ante cambio de pagina. Circuito de Remitos devolución y ventas listo.
</commit_message>
<xml_diff>
--- a/DOCS/REMITO_Master.xlsx
+++ b/DOCS/REMITO_Master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WORKS\CAPELLO SOMBREROS\APPLICATION\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A223510-EEC2-4B2C-9591-D7F85F9CBE1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBC4ED2-CE68-4FA0-B5AF-F194EDB63983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1361,6 +1361,7 @@
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="41">
+        <f>SUM(F10:F34)</f>
         <v>0</v>
       </c>
       <c r="H36" s="26"/>
@@ -1373,7 +1374,7 @@
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="41">
-        <f>SUM(G12:G34)</f>
+        <f>SUM(G10:G34)</f>
         <v>0</v>
       </c>
       <c r="F37" s="1"/>
@@ -1473,8 +1474,8 @@
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="36"/>
-      <c r="F46" s="40"/>
-      <c r="G46" s="40"/>
+      <c r="F46" s="48"/>
+      <c r="G46" s="48"/>
       <c r="H46" s="5"/>
     </row>
     <row r="47" spans="1:44" x14ac:dyDescent="0.25">
@@ -1529,7 +1530,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="E35 E37" unlockedFormula="1"/>
+    <ignoredError sqref="E35:E37" unlockedFormula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>